<commit_message>
fix: ajuste de caminhos e layout da tela de login
</commit_message>
<xml_diff>
--- a/data/usuarios.xlsx
+++ b/data/usuarios.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://giroprodutos-my.sharepoint.com/personal/cig360_giroprodutos_onmicrosoft_com/Documents/COMPARTILHADA - CIG360/02_RELATORIOS/09_PYTHON/ACESSO_WEB/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://giroprodutos-my.sharepoint.com/personal/cig360_giroprodutos_onmicrosoft_com/Documents/COMPARTILHADA - CIG360/02_RELATORIOS/09_PYTHON/ACESSO_WEB/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_AB0D84AFCDF66FFC05FC9890E2EFB2F594FB984F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B16BA60F-8C34-4047-98E0-084DEBA8FC56}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="11_AB0D84AFCDF66FFC05FC9890E2EFB2F594FB984F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{709CE014-D887-40B2-8A4E-56D876B864C4}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>usuario_id</t>
   </si>
@@ -47,9 +47,6 @@
   </si>
   <si>
     <t>maria@teste.com</t>
-  </si>
-  <si>
-    <t>123</t>
   </si>
   <si>
     <t>abc</t>
@@ -114,11 +111,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,7 +424,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,7 +432,7 @@
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.5703125" customWidth="1"/>
     <col min="3" max="3" width="45.28515625" customWidth="1"/>
-    <col min="4" max="4" width="30.140625" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -465,11 +463,11 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
-        <v>9</v>
+      <c r="D2" s="2">
+        <v>123</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -483,10 +481,10 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
         <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>